<commit_message>
Import an Flow excel file should be idempotent close #53
</commit_message>
<xml_diff>
--- a/src/test/javascript/cypress/fixtures/02-import-flows.xlsx
+++ b/src/test/javascript/cypress/fixtures/02-import-flows.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t xml:space="preserve">From ADD</t>
   </si>
@@ -83,6 +83,9 @@
     <t xml:space="preserve">Alias flow</t>
   </si>
   <si>
+    <t xml:space="preserve">External</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source Element</t>
   </si>
   <si>
@@ -192,6 +195,21 @@
   </si>
   <si>
     <t xml:space="preserve">Description TRAD.001 – STEP 04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTERNAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTHER</t>
   </si>
 </sst>
 </file>
@@ -423,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C1:T1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="C1:T1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D1:U1" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="D1:U1"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Source Element"/>
     <tableColumn id="2" name="Target Element"/>
@@ -459,7 +477,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.12"/>
   </cols>
@@ -600,33 +618,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="63.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="24.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,15 +709,15 @@
       <c r="T1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -713,22 +732,22 @@
       <c r="G2" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>47</v>
@@ -737,24 +756,24 @@
         <v>48</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>51</v>
@@ -763,36 +782,68 @@
         <v>52</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>55</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>